<commit_message>
OPT major improvements of push forwarding
</commit_message>
<xml_diff>
--- a/doc/activity_messaging.xlsx
+++ b/doc/activity_messaging.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="190">
   <si>
     <t>Activity / Action</t>
   </si>
@@ -468,6 +468,9 @@
     <t>TODO</t>
   </si>
   <si>
+    <t>{USER} has accepted your friend request</t>
+  </si>
+  <si>
     <t>group membership established</t>
   </si>
   <si>
@@ -480,33 +483,69 @@
     <t>You joined the group: {TITLE}</t>
   </si>
   <si>
+    <t>{USER} has accepted your invitation to the group: {TITLE}</t>
+  </si>
+  <si>
     <t>deleted slot</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>delete</t>
   </si>
   <si>
+    <t>You deleted the Slot: {TITLE}</t>
+  </si>
+  <si>
     <t>{USER} deleted the Slot: {TITLE}</t>
   </si>
   <si>
+    <t>deleted reslot</t>
+  </si>
+  <si>
+    <t>unslot</t>
+  </si>
+  <si>
+    <t>You removed the Reslot: {TITLE}</t>
+  </si>
+  <si>
+    <t>{USER} removed the Reslot: {TITLE}</t>
+  </si>
+  <si>
+    <t>friend request</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>You sended a friend request to you</t>
+  </si>
+  <si>
+    <t>{USER} sended a friend request to you</t>
+  </si>
+  <si>
+    <t>visibility change of slot (user makes public slot private)</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>You unshared the Slot: {TITLE}</t>
+  </si>
+  <si>
+    <t>{USER} unshared the Slot: {TITLE}</t>
+  </si>
+  <si>
     <t>jetzt kommt einfach mal so brainstorm maessig was sonst noch so denkbar waere. manche davon werden wir bewusst nicht machen wollen, aber sicher trotzdem gut, sie explizit auszuschliessen.</t>
   </si>
   <si>
     <t>update existing slot (title, place, start, end)</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>update</t>
   </si>
   <si>
-    <t>deleted reslot</t>
-  </si>
-  <si>
-    <t>unslot</t>
-  </si>
-  <si>
     <t>unliked slot</t>
   </si>
   <si>
@@ -540,12 +579,6 @@
     <t>invite</t>
   </si>
   <si>
-    <t>friend request</t>
-  </si>
-  <si>
-    <t>request</t>
-  </si>
-  <si>
     <t>like a activity</t>
   </si>
   <si>
@@ -579,10 +612,10 @@
     <t>info</t>
   </si>
   <si>
-    <t>visibility change of slot (friend makes privat slot public, ...)</t>
-  </si>
-  <si>
-    <t>visibility</t>
+    <t>visibility change of slot (user makes privat slot public)</t>
+  </si>
+  <si>
+    <t>public</t>
   </si>
   <si>
     <t>friend deactivates his account/ profile</t>
@@ -622,7 +655,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -640,14 +673,7 @@
       <color rgb="FFFF0000"/>
     </font>
     <font>
-      <color rgb="FFFFFFFF"/>
-    </font>
-    <font>
       <i/>
-    </font>
-    <font>
-      <b/>
-      <color rgb="FFFF0000"/>
     </font>
     <font>
       <b/>
@@ -848,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -926,31 +952,17 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
@@ -958,7 +970,7 @@
     <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1012,7 +1024,7 @@
     <col customWidth="1" min="7" max="7" width="38.43"/>
     <col customWidth="1" min="8" max="8" width="34.71"/>
     <col customWidth="1" min="9" max="9" width="42.43"/>
-    <col customWidth="1" min="10" max="10" width="41.86"/>
+    <col customWidth="1" min="10" max="10" width="51.14"/>
     <col customWidth="1" min="11" max="11" width="46.14"/>
     <col customWidth="1" min="12" max="12" width="53.43"/>
     <col customWidth="1" min="13" max="13" width="52.86"/>
@@ -1551,11 +1563,11 @@
       <c r="H13" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="I13" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="J13" s="26" t="s">
-        <v>128</v>
+      <c r="I13" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="K13" s="26" t="s">
         <v>128</v>
@@ -1578,30 +1590,30 @@
     </row>
     <row r="14">
       <c r="A14" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B14" s="19">
         <v>0.8</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H14" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="J14" s="26" t="s">
-        <v>128</v>
+      <c r="I14" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>134</v>
       </c>
       <c r="K14" s="26" t="s">
         <v>128</v>
@@ -1624,28 +1636,30 @@
     </row>
     <row r="15">
       <c r="A15" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="B15" s="22"/>
+        <v>135</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>136</v>
+      </c>
       <c r="C15" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
-      <c r="G15" s="26" t="s">
-        <v>128</v>
+      <c r="G15" s="22" t="s">
+        <v>138</v>
       </c>
       <c r="H15" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="I15" s="26" t="s">
-        <v>128</v>
+      <c r="I15" s="22" t="s">
+        <v>139</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="K15" s="26" t="s">
         <v>128</v>
@@ -1667,187 +1681,281 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
+      <c r="A16" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="N16" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="O16" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="P16" s="26" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
+      <c r="A17" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="L17" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="M17" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="N17" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="O17" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="P17" s="26" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="18">
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="33" t="s">
+      <c r="A18" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C20" s="35" t="s">
+      <c r="C18" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
+      <c r="D18" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="L18" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="N18" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="O18" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="P18" s="26" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C21" s="35" t="s">
+      <c r="A21" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
+      <c r="D22" s="27" t="s">
+        <v>154</v>
+      </c>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
     </row>
     <row r="23">
-      <c r="A23" s="18" t="s">
-        <v>142</v>
+      <c r="A23" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C23" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="36" t="s">
-        <v>143</v>
+      <c r="D23" s="27" t="s">
+        <v>141</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
     </row>
     <row r="24">
       <c r="A24" s="18" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="36" t="s">
-        <v>145</v>
+        <v>136</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>156</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
     </row>
     <row r="25">
       <c r="A25" s="18" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>145</v>
+        <v>136</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>158</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
     </row>
     <row r="26">
-      <c r="A26" s="34" t="s">
-        <v>147</v>
+      <c r="A26" s="18" t="s">
+        <v>159</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>148</v>
+        <v>136</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>158</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
     </row>
     <row r="27">
-      <c r="A27" s="34" t="s">
-        <v>149</v>
+      <c r="A27" s="30" t="s">
+        <v>160</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>150</v>
+        <v>136</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>161</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
     </row>
     <row r="28">
-      <c r="A28" s="34" t="s">
-        <v>151</v>
+      <c r="A28" s="30" t="s">
+        <v>162</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>152</v>
+        <v>136</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>163</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
     </row>
     <row r="29">
-      <c r="A29" s="34" t="s">
-        <v>153</v>
+      <c r="A29" s="30" t="s">
+        <v>164</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>154</v>
+        <v>136</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>165</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
     </row>
     <row r="30">
       <c r="A30" s="18" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="27" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="19"/>
@@ -1855,15 +1963,15 @@
     </row>
     <row r="31">
       <c r="A31" s="18" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="27" t="s">
         <v>31</v>
       </c>
       <c r="E31" s="19"/>
@@ -1871,15 +1979,15 @@
     </row>
     <row r="32">
       <c r="A32" s="18" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C32" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="27" t="s">
         <v>31</v>
       </c>
       <c r="E32" s="19"/>
@@ -1887,15 +1995,15 @@
     </row>
     <row r="33">
       <c r="A33" s="18" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C33" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="27" t="s">
         <v>31</v>
       </c>
       <c r="E33" s="19"/>
@@ -1903,159 +2011,159 @@
     </row>
     <row r="34">
       <c r="A34" s="18" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C34" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="36" t="s">
-        <v>139</v>
+      <c r="D34" s="27" t="s">
+        <v>154</v>
       </c>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
     </row>
     <row r="35">
       <c r="A35" s="18" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="36" t="s">
-        <v>162</v>
+      <c r="D35" s="27" t="s">
+        <v>173</v>
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
     </row>
     <row r="36">
       <c r="A36" s="18" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C36" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D36" s="36" t="s">
-        <v>162</v>
+        <v>136</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>173</v>
       </c>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C37" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="36" t="s">
-        <v>165</v>
+      <c r="D37" s="27" t="s">
+        <v>176</v>
       </c>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
     </row>
     <row r="38">
       <c r="A38" s="18" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C38" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="36" t="s">
-        <v>167</v>
+      <c r="D38" s="27" t="s">
+        <v>178</v>
       </c>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
     </row>
     <row r="39">
       <c r="A39" s="18" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="36" t="s">
-        <v>169</v>
+      <c r="D39" s="27" t="s">
+        <v>180</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
     </row>
     <row r="40">
       <c r="A40" s="18" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C40" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="36" t="s">
-        <v>171</v>
+      <c r="D40" s="27" t="s">
+        <v>182</v>
       </c>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
     </row>
     <row r="41">
-      <c r="A41" s="34" t="s">
-        <v>172</v>
+      <c r="A41" s="30" t="s">
+        <v>183</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="C41" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" s="36" t="s">
-        <v>173</v>
+        <v>136</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>184</v>
       </c>
       <c r="E41" s="19"/>
       <c r="F41" s="19"/>
     </row>
     <row r="42">
-      <c r="C42" s="37"/>
-      <c r="D42" s="38"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="32"/>
     </row>
     <row r="43">
-      <c r="C43" s="39" t="s">
-        <v>174</v>
+      <c r="C43" s="33" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="33" t="s">
-        <v>175</v>
+      <c r="A44" s="29" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="22" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="22" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="33" t="s">
-        <v>178</v>
+      <c r="A48" s="29" t="s">
+        <v>189</v>
       </c>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
@@ -3049,7 +3157,7 @@
       </c>
       <c r="B102" t="str">
         <f>""""&amp;SUBSTITUTE(Definition!I13, "{", "%{")&amp;""""</f>
-        <v>"TODO"</v>
+        <v>"You and %{USER} are now friends"</v>
       </c>
     </row>
     <row r="103">
@@ -3059,7 +3167,7 @@
       </c>
       <c r="B103" t="str">
         <f>""""&amp;SUBSTITUTE(Definition!J13, "{", "%{")&amp;""""</f>
-        <v>"TODO"</v>
+        <v>"%{USER} has accepted your friend request"</v>
       </c>
     </row>
     <row r="104">
@@ -3149,7 +3257,7 @@
       </c>
       <c r="B113" t="str">
         <f>""""&amp;SUBSTITUTE(Definition!I14, "{", "%{")&amp;""""</f>
-        <v>"TODO"</v>
+        <v>"You joined the group: %{TITLE}"</v>
       </c>
     </row>
     <row r="114">
@@ -3159,7 +3267,7 @@
       </c>
       <c r="B114" t="str">
         <f>""""&amp;SUBSTITUTE(Definition!J14, "{", "%{")&amp;""""</f>
-        <v>"TODO"</v>
+        <v>"%{USER} has accepted your invitation to the group: %{TITLE}"</v>
       </c>
     </row>
     <row r="115">
@@ -3229,7 +3337,7 @@
       </c>
       <c r="B122" t="str">
         <f>""""&amp;SUBSTITUTE(Definition!G15, "{", "%{")&amp;""""</f>
-        <v>"TODO"</v>
+        <v>"You deleted the Slot: %{TITLE}"</v>
       </c>
     </row>
     <row r="123">
@@ -3249,7 +3357,7 @@
       </c>
       <c r="B124" t="str">
         <f>""""&amp;SUBSTITUTE(Definition!I15, "{", "%{")&amp;""""</f>
-        <v>"TODO"</v>
+        <v>"%{USER} deleted the Slot: %{TITLE}"</v>
       </c>
     </row>
     <row r="125">
@@ -3319,6 +3427,306 @@
       </c>
       <c r="B131" t="str">
         <f>""""&amp;SUBSTITUTE(Definition!P15, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$G$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>slot_unslot_me_singular:</v>
+      </c>
+      <c r="B133" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!G16, "{", "%{")&amp;""""</f>
+        <v>"You removed the Reslot: %{TITLE}"</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$H$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>slot_unslot_activity_singular:</v>
+      </c>
+      <c r="B134" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!H16, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$I$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>slot_unslot_notify_singular:</v>
+      </c>
+      <c r="B135" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!I16, "{", "%{")&amp;""""</f>
+        <v>"%{USER} removed the Reslot: %{TITLE}"</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$J$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>slot_unslot_push_singular:</v>
+      </c>
+      <c r="B136" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!J16, "{", "%{")&amp;""""</f>
+        <v>"%{USER} removed the Reslot: %{TITLE}"</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$K$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>slot_unslot_activity_plural:</v>
+      </c>
+      <c r="B137" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!K16, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$L$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>slot_unslot_notify_plural:</v>
+      </c>
+      <c r="B138" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!L16, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$M$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>slot_unslot_push_plural:</v>
+      </c>
+      <c r="B139" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!M16, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$N$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>slot_unslot_activity_aggregate:</v>
+      </c>
+      <c r="B140" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!N16, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$O$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>slot_unslot_notify_aggregate:</v>
+      </c>
+      <c r="B141" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!O16, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <f>LOWER(Definition!C16&amp;"_"&amp;Definition!D16&amp;"_"&amp;Definition!$P$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>slot_unslot_push_aggregate:</v>
+      </c>
+      <c r="B142" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!P16, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$G$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>user_request_me_singular:</v>
+      </c>
+      <c r="B144" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!G17, "{", "%{")&amp;""""</f>
+        <v>"You sended a friend request to you"</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$H$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>user_request_activity_singular:</v>
+      </c>
+      <c r="B145" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!H17, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$I$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>user_request_notify_singular:</v>
+      </c>
+      <c r="B146" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!I17, "{", "%{")&amp;""""</f>
+        <v>"%{USER} sended a friend request to you"</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$J$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>user_request_push_singular:</v>
+      </c>
+      <c r="B147" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!J17, "{", "%{")&amp;""""</f>
+        <v>"%{USER} sended a friend request to you"</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$K$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>user_request_activity_plural:</v>
+      </c>
+      <c r="B148" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!K17, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$L$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>user_request_notify_plural:</v>
+      </c>
+      <c r="B149" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!L17, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$M$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>user_request_push_plural:</v>
+      </c>
+      <c r="B150" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!M17, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$N$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>user_request_activity_aggregate:</v>
+      </c>
+      <c r="B151" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!N17, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$O$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>user_request_notify_aggregate:</v>
+      </c>
+      <c r="B152" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!O17, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <f>LOWER(Definition!C17&amp;"_"&amp;Definition!D17&amp;"_"&amp;Definition!$P$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>user_request_push_aggregate:</v>
+      </c>
+      <c r="B153" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!P17, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$G$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>slot_private_me_singular:</v>
+      </c>
+      <c r="B155" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!G18, "{", "%{")&amp;""""</f>
+        <v>"You unshared the Slot: %{TITLE}"</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$H$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>slot_private_activity_singular:</v>
+      </c>
+      <c r="B156" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!H18, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$I$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>slot_private_notify_singular:</v>
+      </c>
+      <c r="B157" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!I18, "{", "%{")&amp;""""</f>
+        <v>"%{USER} unshared the Slot: %{TITLE}"</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$J$3&amp;"_"&amp;Definition!$G$2&amp;":")</f>
+        <v>slot_private_push_singular:</v>
+      </c>
+      <c r="B158" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!J18, "{", "%{")&amp;""""</f>
+        <v>"%{USER} unshared the Slot: %{TITLE}"</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$K$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>slot_private_activity_plural:</v>
+      </c>
+      <c r="B159" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!K18, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$L$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>slot_private_notify_plural:</v>
+      </c>
+      <c r="B160" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!L18, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$M$3&amp;"_"&amp;Definition!$K$2&amp;":")</f>
+        <v>slot_private_push_plural:</v>
+      </c>
+      <c r="B161" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!M18, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$N$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>slot_private_activity_aggregate:</v>
+      </c>
+      <c r="B162" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!N18, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$O$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>slot_private_notify_aggregate:</v>
+      </c>
+      <c r="B163" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!O18, "{", "%{")&amp;""""</f>
+        <v>"TODO"</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <f>LOWER(Definition!C18&amp;"_"&amp;Definition!D18&amp;"_"&amp;Definition!$P$3&amp;"_"&amp;Definition!$N$2&amp;":")</f>
+        <v>slot_private_push_aggregate:</v>
+      </c>
+      <c r="B164" t="str">
+        <f>""""&amp;SUBSTITUTE(Definition!P18, "{", "%{")&amp;""""</f>
         <v>"TODO"</v>
       </c>
     </row>

</xml_diff>